<commit_message>
made color-parser more robust and added excel with all picked values
</commit_message>
<xml_diff>
--- a/test2-colors/hue20.xlsx
+++ b/test2-colors/hue20.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L361"/>
+  <dimension ref="A1:L362"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,140 +473,140 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>#cb6e17</t>
+          <t>#176ecb</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="L3" t="inlineStr">
         <is>
-          <t>#d06400</t>
+          <t>#0064d0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="L4" t="inlineStr">
         <is>
-          <t>#ce5300</t>
+          <t>#0053ce</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="L5" t="inlineStr">
         <is>
-          <t>#de6a00</t>
+          <t>#006ade</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="L6" t="inlineStr">
         <is>
-          <t>#d98400</t>
+          <t>#0084d9</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="L7" t="inlineStr">
         <is>
-          <t>#efbe04</t>
+          <t>#04beef</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="L8" t="inlineStr">
         <is>
-          <t>#b47b00</t>
+          <t>#007bb4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="L9" t="inlineStr">
         <is>
-          <t>#d9a909</t>
+          <t>#09a9d9</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="L10" t="inlineStr">
         <is>
-          <t>#b48200</t>
+          <t>#0082b4</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="L11" t="inlineStr">
         <is>
-          <t>#e8c119</t>
+          <t>#19c1e8</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="L12" t="inlineStr">
         <is>
-          <t>#dcba0d</t>
+          <t>#0dbadc</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="L13" t="inlineStr">
         <is>
-          <t>#bd9402</t>
+          <t>#0294bd</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="L14" t="inlineStr">
         <is>
-          <t>#ae8605</t>
+          <t>#0586ae</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="L15" t="inlineStr">
         <is>
-          <t>#e7ce1a</t>
+          <t>#1acee7</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="L16" t="inlineStr">
         <is>
-          <t>#e2c723</t>
+          <t>#23c7e2</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="L17" t="inlineStr">
         <is>
-          <t>#c1990a</t>
+          <t>#0a99c1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="L18" t="inlineStr">
         <is>
-          <t>#b37a00</t>
+          <t>#007ab3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="L19" t="inlineStr">
         <is>
-          <t>#e4b107</t>
+          <t>#07b1e4</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="L20" t="inlineStr">
         <is>
-          <t>#f3b608</t>
+          <t>#08b6f3</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="L21" t="inlineStr">
         <is>
-          <t>#ce9100</t>
+          <t>#0091ce</t>
         </is>
       </c>
     </row>
@@ -668,140 +668,140 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>#3b61ef</t>
+          <t>#ef613b</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="L23" t="inlineStr">
         <is>
-          <t>#4264f3</t>
+          <t>#f36442</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="L24" t="inlineStr">
         <is>
-          <t>#1c3bd2</t>
+          <t>#d23b1c</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="L25" t="inlineStr">
         <is>
-          <t>#303b9d</t>
+          <t>#9d3b30</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="L26" t="inlineStr">
         <is>
-          <t>#1a35c5</t>
+          <t>#c5351a</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="L27" t="inlineStr">
         <is>
-          <t>#1131ca</t>
+          <t>#ca3111</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="L28" t="inlineStr">
         <is>
-          <t>#2946dd</t>
+          <t>#dd4629</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="L29" t="inlineStr">
         <is>
-          <t>#626de6</t>
+          <t>#e66d62</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="L30" t="inlineStr">
         <is>
-          <t>#556eee</t>
+          <t>#ee6e55</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="L31" t="inlineStr">
         <is>
-          <t>#515ddb</t>
+          <t>#db5d51</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="L32" t="inlineStr">
         <is>
-          <t>#2041d6</t>
+          <t>#d64120</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="L33" t="inlineStr">
         <is>
-          <t>#3f65ed</t>
+          <t>#ed653f</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="L34" t="inlineStr">
         <is>
-          <t>#6e80d9</t>
+          <t>#d9806e</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="L35" t="inlineStr">
         <is>
-          <t>#2d49cc</t>
+          <t>#cc492d</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="L36" t="inlineStr">
         <is>
-          <t>#363fbe</t>
+          <t>#be3f36</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="L37" t="inlineStr">
         <is>
-          <t>#6468de</t>
+          <t>#de6864</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="L38" t="inlineStr">
         <is>
-          <t>#3c5ae7</t>
+          <t>#e75a3c</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="L39" t="inlineStr">
         <is>
-          <t>#1d43df</t>
+          <t>#df431d</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="L40" t="inlineStr">
         <is>
-          <t>#3f5ce7</t>
+          <t>#e75c3f</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="L41" t="inlineStr">
         <is>
-          <t>#2d43c5</t>
+          <t>#c5432d</t>
         </is>
       </c>
     </row>
@@ -863,140 +863,140 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>#d74dd4</t>
+          <t>#d44dd7</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="L43" t="inlineStr">
         <is>
-          <t>#ee6ce9</t>
+          <t>#e96cee</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="L44" t="inlineStr">
         <is>
-          <t>#eb6ae9</t>
+          <t>#e96aeb</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="L45" t="inlineStr">
         <is>
-          <t>#d959e0</t>
+          <t>#e059d9</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="L46" t="inlineStr">
         <is>
-          <t>#d758dd</t>
+          <t>#dd58d7</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="L47" t="inlineStr">
         <is>
-          <t>#cf48c6</t>
+          <t>#c648cf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="L48" t="inlineStr">
         <is>
-          <t>#eb68db</t>
+          <t>#db68eb</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="L49" t="inlineStr">
         <is>
-          <t>#f079db</t>
+          <t>#db79f0</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="L50" t="inlineStr">
         <is>
-          <t>#ea6ad3</t>
+          <t>#d36aea</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="L51" t="inlineStr">
         <is>
-          <t>#b53681</t>
+          <t>#8136b5</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="L52" t="inlineStr">
         <is>
-          <t>#a63273</t>
+          <t>#7332a6</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="L53" t="inlineStr">
         <is>
-          <t>#bf3e81</t>
+          <t>#813ebf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="L54" t="inlineStr">
         <is>
-          <t>#da5da7</t>
+          <t>#a75dda</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="L55" t="inlineStr">
         <is>
-          <t>#d653aa</t>
+          <t>#aa53d6</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="L56" t="inlineStr">
         <is>
-          <t>#ac3988</t>
+          <t>#8839ac</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="L57" t="inlineStr">
         <is>
-          <t>#a72f8e</t>
+          <t>#8e2fa7</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="L58" t="inlineStr">
         <is>
-          <t>#9b3293</t>
+          <t>#93329b</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="L59" t="inlineStr">
         <is>
-          <t>#8147a6</t>
+          <t>#a64781</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="L60" t="inlineStr">
         <is>
-          <t>#a74ecd</t>
+          <t>#cd4ea7</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="L61" t="inlineStr">
         <is>
-          <t>#b64bdd</t>
+          <t>#dd4bb6</t>
         </is>
       </c>
     </row>
@@ -1058,140 +1058,140 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>#3c56f0</t>
+          <t>#f0563c</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="L63" t="inlineStr">
         <is>
-          <t>#9254ee</t>
+          <t>#ee5492</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="L64" t="inlineStr">
         <is>
-          <t>#b54bda</t>
+          <t>#da4bb5</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="L65" t="inlineStr">
         <is>
-          <t>#d76def</t>
+          <t>#ef6dd7</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="L66" t="inlineStr">
         <is>
-          <t>#d36ff1</t>
+          <t>#f16fd3</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="L67" t="inlineStr">
         <is>
-          <t>#ae56e9</t>
+          <t>#e956ae</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="L68" t="inlineStr">
         <is>
-          <t>#465dd7</t>
+          <t>#d75d46</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="L69" t="inlineStr">
         <is>
-          <t>#3e4dea</t>
+          <t>#ea4d3e</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="L70" t="inlineStr">
         <is>
-          <t>#3b4de8</t>
+          <t>#e84d3b</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="L71" t="inlineStr">
         <is>
-          <t>#8142de</t>
+          <t>#de4281</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="L72" t="inlineStr">
         <is>
-          <t>#1932c8</t>
+          <t>#c83219</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="L73" t="inlineStr">
         <is>
-          <t>#8450ea</t>
+          <t>#ea5084</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="L74" t="inlineStr">
         <is>
-          <t>#8120b6</t>
+          <t>#b62081</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="L75" t="inlineStr">
         <is>
-          <t>#e177ef</t>
+          <t>#ef77e1</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="L76" t="inlineStr">
         <is>
-          <t>#c25ce9</t>
+          <t>#e95cc2</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="L77" t="inlineStr">
         <is>
-          <t>#aa43c2</t>
+          <t>#c243aa</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="L78" t="inlineStr">
         <is>
-          <t>#6c30c4</t>
+          <t>#c4306c</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="L79" t="inlineStr">
         <is>
-          <t>#3f4de6</t>
+          <t>#e64d3f</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="L80" t="inlineStr">
         <is>
-          <t>#3f4de6</t>
+          <t>#e64d3f</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="L81" t="inlineStr">
         <is>
-          <t>#5063d6</t>
+          <t>#d66350</t>
         </is>
       </c>
     </row>
@@ -1253,140 +1253,140 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>#9e9fd9</t>
+          <t>#d99f9e</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="L83" t="inlineStr">
         <is>
-          <t>#7779d7</t>
+          <t>#d77977</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="L84" t="inlineStr">
         <is>
-          <t>#826ad6</t>
+          <t>#d66a82</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="L85" t="inlineStr">
         <is>
-          <t>#6585d8</t>
+          <t>#d88565</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="L86" t="inlineStr">
         <is>
-          <t>#b9dbeb</t>
+          <t>#ebdbb9</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="L87" t="inlineStr">
         <is>
-          <t>#6ca2d1</t>
+          <t>#d1a26c</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="L88" t="inlineStr">
         <is>
-          <t>#8d9275</t>
+          <t>#75928d</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="L89" t="inlineStr">
         <is>
-          <t>#c7d1c4</t>
+          <t>#c4d1c7</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="L90" t="inlineStr">
         <is>
-          <t>#d6f9ff</t>
+          <t>#fff9d6</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="L91" t="inlineStr">
         <is>
-          <t>#93b9c5</t>
+          <t>#c5b993</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="L92" t="inlineStr">
         <is>
-          <t>#5e73cf</t>
+          <t>#cf735e</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="L93" t="inlineStr">
         <is>
-          <t>#7ba6b5</t>
+          <t>#b5a67b</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="L94" t="inlineStr">
         <is>
-          <t>#8a80e4</t>
+          <t>#e4808a</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="L95" t="inlineStr">
         <is>
-          <t>#7782d2</t>
+          <t>#d28277</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="L96" t="inlineStr">
         <is>
-          <t>#bd8dd5</t>
+          <t>#d58dbd</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="L97" t="inlineStr">
         <is>
-          <t>#eacfcb</t>
+          <t>#cbcfea</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="L98" t="inlineStr">
         <is>
-          <t>#947ecc</t>
+          <t>#cc7e94</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="L99" t="inlineStr">
         <is>
-          <t>#6b90ca</t>
+          <t>#ca906b</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="L100" t="inlineStr">
         <is>
-          <t>#7672db</t>
+          <t>#db7276</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="L101" t="inlineStr">
         <is>
-          <t>#548acb</t>
+          <t>#cb8a54</t>
         </is>
       </c>
     </row>
@@ -1448,140 +1448,140 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>#0e7364</t>
+          <t>#64730e</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="L103" t="inlineStr">
         <is>
-          <t>#5dd3a3</t>
+          <t>#a3d35d</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="L104" t="inlineStr">
         <is>
-          <t>#208075</t>
+          <t>#758020</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="L105" t="inlineStr">
         <is>
-          <t>#0a6e68</t>
+          <t>#686e0a</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="L106" t="inlineStr">
         <is>
-          <t>#136062</t>
+          <t>#626013</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="L107" t="inlineStr">
         <is>
-          <t>#47b49e</t>
+          <t>#9eb447</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="L108" t="inlineStr">
         <is>
-          <t>#005d49</t>
+          <t>#495d00</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="L109" t="inlineStr">
         <is>
-          <t>#186e62</t>
+          <t>#626e18</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="L110" t="inlineStr">
         <is>
-          <t>#146d5d</t>
+          <t>#5d6d14</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="L111" t="inlineStr">
         <is>
-          <t>#005e42</t>
+          <t>#425e00</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="L112" t="inlineStr">
         <is>
-          <t>#066b55</t>
+          <t>#556b06</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="L113" t="inlineStr">
         <is>
-          <t>#4a826b</t>
+          <t>#6b824a</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="L114" t="inlineStr">
         <is>
-          <t>#094239</t>
+          <t>#394209</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="L115" t="inlineStr">
         <is>
-          <t>#4f9480</t>
+          <t>#80944f</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="L116" t="inlineStr">
         <is>
-          <t>#227b89</t>
+          <t>#897b22</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="L117" t="inlineStr">
         <is>
-          <t>#105548</t>
+          <t>#485510</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="L118" t="inlineStr">
         <is>
-          <t>#168275</t>
+          <t>#758216</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="L119" t="inlineStr">
         <is>
-          <t>#1a6555</t>
+          <t>#55651a</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="L120" t="inlineStr">
         <is>
-          <t>#0d594d</t>
+          <t>#4d590d</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="L121" t="inlineStr">
         <is>
-          <t>#207d7e</t>
+          <t>#7e7d20</t>
         </is>
       </c>
     </row>
@@ -1643,140 +1643,140 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>#e89c5a</t>
+          <t>#5a9ce8</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="L123" t="inlineStr">
         <is>
-          <t>#dc700a</t>
+          <t>#0a70dc</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="L124" t="inlineStr">
         <is>
-          <t>#ff8703</t>
+          <t>#0387ff</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="L125" t="inlineStr">
         <is>
-          <t>#eeab02</t>
+          <t>#02abee</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="L126" t="inlineStr">
         <is>
-          <t>#fd8e04</t>
+          <t>#048efd</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="L127" t="inlineStr">
         <is>
-          <t>#f1b700</t>
+          <t>#00b7f1</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="L128" t="inlineStr">
         <is>
-          <t>#eb7c00</t>
+          <t>#007ceb</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="L129" t="inlineStr">
         <is>
-          <t>#cd7d02</t>
+          <t>#027dcd</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="L130" t="inlineStr">
         <is>
-          <t>#cd4e00</t>
+          <t>#004ecd</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="L131" t="inlineStr">
         <is>
-          <t>#d64200</t>
+          <t>#0042d6</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="L132" t="inlineStr">
         <is>
-          <t>#f86802</t>
+          <t>#0268f8</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="L133" t="inlineStr">
         <is>
-          <t>#fd7303</t>
+          <t>#0373fd</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="L134" t="inlineStr">
         <is>
-          <t>#e57c33</t>
+          <t>#337ce5</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="L135" t="inlineStr">
         <is>
-          <t>#db9353</t>
+          <t>#5393db</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="L136" t="inlineStr">
         <is>
-          <t>#ac4900</t>
+          <t>#0049ac</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="L137" t="inlineStr">
         <is>
-          <t>#a15a10</t>
+          <t>#105aa1</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="L138" t="inlineStr">
         <is>
-          <t>#f1ad00</t>
+          <t>#00adf1</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="L139" t="inlineStr">
         <is>
-          <t>#fe9700</t>
+          <t>#0097fe</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="L140" t="inlineStr">
         <is>
-          <t>#ebb203</t>
+          <t>#03b2eb</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="L141" t="inlineStr">
         <is>
-          <t>#ffb00a</t>
+          <t>#0ab0ff</t>
         </is>
       </c>
     </row>
@@ -1838,140 +1838,140 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>#7d97cd</t>
+          <t>#cd977d</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="L143" t="inlineStr">
         <is>
-          <t>#a0b1c4</t>
+          <t>#c4b1a0</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="L144" t="inlineStr">
         <is>
-          <t>#77598e</t>
+          <t>#8e5977</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="L145" t="inlineStr">
         <is>
-          <t>#724e78</t>
+          <t>#784e72</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="L146" t="inlineStr">
         <is>
-          <t>#538994</t>
+          <t>#948953</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="L147" t="inlineStr">
         <is>
-          <t>#478a7b</t>
+          <t>#7b8a47</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="L148" t="inlineStr">
         <is>
-          <t>#9edad2</t>
+          <t>#d2da9e</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="L149" t="inlineStr">
         <is>
-          <t>#a0c299</t>
+          <t>#99c2a0</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="L150" t="inlineStr">
         <is>
-          <t>#95ad73</t>
+          <t>#73ad95</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="L151" t="inlineStr">
         <is>
-          <t>#637948</t>
+          <t>#487963</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="L152" t="inlineStr">
         <is>
-          <t>#3d6647</t>
+          <t>#47663d</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="L153" t="inlineStr">
         <is>
-          <t>#3e7086</t>
+          <t>#86703e</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="L154" t="inlineStr">
         <is>
-          <t>#454575</t>
+          <t>#754545</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="L155" t="inlineStr">
         <is>
-          <t>#4e4685</t>
+          <t>#85464e</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="L156" t="inlineStr">
         <is>
-          <t>#595ca0</t>
+          <t>#a05c59</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="L157" t="inlineStr">
         <is>
-          <t>#8ab3d4</t>
+          <t>#d4b38a</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="L158" t="inlineStr">
         <is>
-          <t>#90d3ce</t>
+          <t>#ced390</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="L159" t="inlineStr">
         <is>
-          <t>#52a3a0</t>
+          <t>#a0a352</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="L160" t="inlineStr">
         <is>
-          <t>#89b1cd</t>
+          <t>#cdb189</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="L161" t="inlineStr">
         <is>
-          <t>#809ecf</t>
+          <t>#cf9e80</t>
         </is>
       </c>
     </row>
@@ -2033,140 +2033,140 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>#f27604</t>
+          <t>#0476f2</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="L163" t="inlineStr">
         <is>
-          <t>#fe901a</t>
+          <t>#1a90fe</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="L164" t="inlineStr">
         <is>
-          <t>#e36b48</t>
+          <t>#486be3</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="L165" t="inlineStr">
         <is>
-          <t>#f27a02</t>
+          <t>#027af2</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="L166" t="inlineStr">
         <is>
-          <t>#f78000</t>
+          <t>#0080f7</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="L167" t="inlineStr">
         <is>
-          <t>#ce6516</t>
+          <t>#1665ce</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="L168" t="inlineStr">
         <is>
-          <t>#d04e0d</t>
+          <t>#0d4ed0</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="L169" t="inlineStr">
         <is>
-          <t>#ec887c</t>
+          <t>#7c88ec</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="L170" t="inlineStr">
         <is>
-          <t>#c5535a</t>
+          <t>#5a53c5</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="L171" t="inlineStr">
         <is>
-          <t>#943036</t>
+          <t>#363094</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="L172" t="inlineStr">
         <is>
-          <t>#c6585e</t>
+          <t>#5e58c6</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="L173" t="inlineStr">
         <is>
-          <t>#d56c75</t>
+          <t>#756cd5</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="L174" t="inlineStr">
         <is>
-          <t>#cc5760</t>
+          <t>#6057cc</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="L175" t="inlineStr">
         <is>
-          <t>#f7892f</t>
+          <t>#2f89f7</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="L176" t="inlineStr">
         <is>
-          <t>#fb8900</t>
+          <t>#0089fb</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="L177" t="inlineStr">
         <is>
-          <t>#d65200</t>
+          <t>#0052d6</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="L178" t="inlineStr">
         <is>
-          <t>#ec7635</t>
+          <t>#3576ec</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="L179" t="inlineStr">
         <is>
-          <t>#f47f00</t>
+          <t>#007ff4</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="L180" t="inlineStr">
         <is>
-          <t>#e46821</t>
+          <t>#2168e4</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="L181" t="inlineStr">
         <is>
-          <t>#b14649</t>
+          <t>#4946b1</t>
         </is>
       </c>
     </row>
@@ -2235,133 +2235,133 @@
     <row r="183">
       <c r="L183" t="inlineStr">
         <is>
-          <t>#1a874f</t>
+          <t>#4f871a</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="L184" t="inlineStr">
         <is>
-          <t>#1a874f</t>
+          <t>#4f871a</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="L185" t="inlineStr">
         <is>
-          <t>#1a874f</t>
+          <t>#4f871a</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="L186" t="inlineStr">
         <is>
-          <t>#1a874f</t>
+          <t>#4f871a</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="L187" t="inlineStr">
         <is>
-          <t>#2aa450</t>
+          <t>#50a42a</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="L188" t="inlineStr">
         <is>
-          <t>#26a556</t>
+          <t>#56a526</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="L189" t="inlineStr">
         <is>
-          <t>#128738</t>
+          <t>#388712</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="L190" t="inlineStr">
         <is>
-          <t>#0f7c4e</t>
+          <t>#4e7c0f</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="L191" t="inlineStr">
         <is>
-          <t>#2f936f</t>
+          <t>#6f932f</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="L192" t="inlineStr">
         <is>
-          <t>#429378</t>
+          <t>#789342</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="L193" t="inlineStr">
         <is>
-          <t>#456b5f</t>
+          <t>#5f6b45</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="L194" t="inlineStr">
         <is>
-          <t>#234e3f</t>
+          <t>#3f4e23</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="L195" t="inlineStr">
         <is>
-          <t>#123d30</t>
+          <t>#303d12</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="L196" t="inlineStr">
         <is>
-          <t>#124a37</t>
+          <t>#374a12</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="L197" t="inlineStr">
         <is>
-          <t>#5f7949</t>
+          <t>#49795f</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="L198" t="inlineStr">
         <is>
-          <t>#2e5e1c</t>
+          <t>#1c5e2e</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="L199" t="inlineStr">
         <is>
-          <t>#1d775a</t>
+          <t>#5a771d</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="L200" t="inlineStr">
         <is>
-          <t>#2fa669</t>
+          <t>#69a62f</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="L201" t="inlineStr">
         <is>
-          <t>#2ba84c</t>
+          <t>#4ca82b</t>
         </is>
       </c>
     </row>
@@ -2423,140 +2423,140 @@
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>#ee810e</t>
+          <t>#0e81ee</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="L203" t="inlineStr">
         <is>
-          <t>#ff8b03</t>
+          <t>#038bff</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="L204" t="inlineStr">
         <is>
-          <t>#de5500</t>
+          <t>#0055de</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="L205" t="inlineStr">
         <is>
-          <t>#f57b00</t>
+          <t>#007bf5</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="L206" t="inlineStr">
         <is>
-          <t>#f46a00</t>
+          <t>#006af4</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="L207" t="inlineStr">
         <is>
-          <t>#e35203</t>
+          <t>#0352e3</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="L208" t="inlineStr">
         <is>
-          <t>#e45000</t>
+          <t>#0050e4</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="L209" t="inlineStr">
         <is>
-          <t>#ff7b01</t>
+          <t>#017bff</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="L210" t="inlineStr">
         <is>
-          <t>#fa7800</t>
+          <t>#0078fa</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="L211" t="inlineStr">
         <is>
-          <t>#e0600d</t>
+          <t>#0d60e0</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="L212" t="inlineStr">
         <is>
-          <t>#d0500f</t>
+          <t>#0f50d0</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="L213" t="inlineStr">
         <is>
-          <t>#d54602</t>
+          <t>#0246d5</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="L214" t="inlineStr">
         <is>
-          <t>#b23005</t>
+          <t>#0530b2</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="L215" t="inlineStr">
         <is>
-          <t>#c53401</t>
+          <t>#0134c5</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="L216" t="inlineStr">
         <is>
-          <t>#ff8c00</t>
+          <t>#008cff</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="L217" t="inlineStr">
         <is>
-          <t>#f86c07</t>
+          <t>#076cf8</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="L218" t="inlineStr">
         <is>
-          <t>#e54b04</t>
+          <t>#044be5</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="L219" t="inlineStr">
         <is>
-          <t>#fb7d00</t>
+          <t>#007dfb</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="L220" t="inlineStr">
         <is>
-          <t>#ff8600</t>
+          <t>#0086ff</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="L221" t="inlineStr">
         <is>
-          <t>#ff8d01</t>
+          <t>#018dff</t>
         </is>
       </c>
     </row>
@@ -2618,140 +2618,140 @@
       </c>
       <c r="L222" t="inlineStr">
         <is>
-          <t>#c53f99</t>
+          <t>#993fc5</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="L223" t="inlineStr">
         <is>
-          <t>#f786d6</t>
+          <t>#d686f7</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="L224" t="inlineStr">
         <is>
-          <t>#da5db9</t>
+          <t>#b95dda</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="L225" t="inlineStr">
         <is>
-          <t>#cf50ab</t>
+          <t>#ab50cf</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="L226" t="inlineStr">
         <is>
-          <t>#d253a2</t>
+          <t>#a253d2</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="L227" t="inlineStr">
         <is>
-          <t>#ef80ca</t>
+          <t>#ca80ef</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="L228" t="inlineStr">
         <is>
-          <t>#e66bc1</t>
+          <t>#c16be6</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="L229" t="inlineStr">
         <is>
-          <t>#d354a9</t>
+          <t>#a954d3</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="L230" t="inlineStr">
         <is>
-          <t>#db5cb2</t>
+          <t>#b25cdb</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="L231" t="inlineStr">
         <is>
-          <t>#d14ea9</t>
+          <t>#a94ed1</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="L232" t="inlineStr">
         <is>
-          <t>#dc5cad</t>
+          <t>#ad5cdc</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="L233" t="inlineStr">
         <is>
-          <t>#e260bf</t>
+          <t>#bf60e2</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="L234" t="inlineStr">
         <is>
-          <t>#db67ba</t>
+          <t>#ba67db</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="L235" t="inlineStr">
         <is>
-          <t>#da5dac</t>
+          <t>#ac5dda</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="L236" t="inlineStr">
         <is>
-          <t>#e060b9</t>
+          <t>#b960e0</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="L237" t="inlineStr">
         <is>
-          <t>#d866a2</t>
+          <t>#a266d8</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="L238" t="inlineStr">
         <is>
-          <t>#cf48a4</t>
+          <t>#a448cf</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="L239" t="inlineStr">
         <is>
-          <t>#d85ab3</t>
+          <t>#b35ad8</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="L240" t="inlineStr">
         <is>
-          <t>#e869be</t>
+          <t>#be69e8</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="L241" t="inlineStr">
         <is>
-          <t>#c745a4</t>
+          <t>#a445c7</t>
         </is>
       </c>
     </row>
@@ -2813,140 +2813,140 @@
       </c>
       <c r="L242" t="inlineStr">
         <is>
-          <t>#dd956d</t>
+          <t>#6d95dd</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="L243" t="inlineStr">
         <is>
-          <t>#e47249</t>
+          <t>#4972e4</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="L244" t="inlineStr">
         <is>
-          <t>#e287b8</t>
+          <t>#b887e2</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="L245" t="inlineStr">
         <is>
-          <t>#e08fc0</t>
+          <t>#c08fe0</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="L246" t="inlineStr">
         <is>
-          <t>#c3699e</t>
+          <t>#9e69c3</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="L247" t="inlineStr">
         <is>
-          <t>#cd6e3c</t>
+          <t>#3c6ecd</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="L248" t="inlineStr">
         <is>
-          <t>#d6643f</t>
+          <t>#3f64d6</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="L249" t="inlineStr">
         <is>
-          <t>#cb5942</t>
+          <t>#4259cb</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="L250" t="inlineStr">
         <is>
-          <t>#c76191</t>
+          <t>#9161c7</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="L251" t="inlineStr">
         <is>
-          <t>#cd7bb0</t>
+          <t>#b07bcd</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="L252" t="inlineStr">
         <is>
-          <t>#9b4b76</t>
+          <t>#764b9b</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="L253" t="inlineStr">
         <is>
-          <t>#b85f62</t>
+          <t>#625fb8</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="L254" t="inlineStr">
         <is>
-          <t>#f6976c</t>
+          <t>#6c97f6</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="L255" t="inlineStr">
         <is>
-          <t>#e47e5b</t>
+          <t>#5b7ee4</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="L256" t="inlineStr">
         <is>
-          <t>#b44a73</t>
+          <t>#734ab4</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="L257" t="inlineStr">
         <is>
-          <t>#b35a8b</t>
+          <t>#8b5ab3</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="L258" t="inlineStr">
         <is>
-          <t>#cb79ad</t>
+          <t>#ad79cb</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="L259" t="inlineStr">
         <is>
-          <t>#954973</t>
+          <t>#734995</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="L260" t="inlineStr">
         <is>
-          <t>#c96773</t>
+          <t>#7367c9</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="L261" t="inlineStr">
         <is>
-          <t>#ed865f</t>
+          <t>#5f86ed</t>
         </is>
       </c>
     </row>
@@ -3008,140 +3008,140 @@
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>#dbd120</t>
+          <t>#20d1db</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="L263" t="inlineStr">
         <is>
-          <t>#dcd129</t>
+          <t>#29d1dc</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="L264" t="inlineStr">
         <is>
-          <t>#99c843</t>
+          <t>#43c899</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="L265" t="inlineStr">
         <is>
-          <t>#50982e</t>
+          <t>#2e9850</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="L266" t="inlineStr">
         <is>
-          <t>#c3e037</t>
+          <t>#37e0c3</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="L267" t="inlineStr">
         <is>
-          <t>#53a02d</t>
+          <t>#2da053</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="L268" t="inlineStr">
         <is>
-          <t>#bdb111</t>
+          <t>#11b1bd</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="L269" t="inlineStr">
         <is>
-          <t>#d7c425</t>
+          <t>#25c4d7</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="L270" t="inlineStr">
         <is>
-          <t>#ceb928</t>
+          <t>#28b9ce</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="L271" t="inlineStr">
         <is>
-          <t>#bbcb26</t>
+          <t>#26cbbb</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="L272" t="inlineStr">
         <is>
-          <t>#b2db2c</t>
+          <t>#2cdbb2</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="L273" t="inlineStr">
         <is>
-          <t>#bfdb34</t>
+          <t>#34dbbf</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="L274" t="inlineStr">
         <is>
-          <t>#bfdb34</t>
+          <t>#34dbbf</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="L275" t="inlineStr">
         <is>
-          <t>#c5c710</t>
+          <t>#10c7c5</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="L276" t="inlineStr">
         <is>
-          <t>#e3d626</t>
+          <t>#26d6e3</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="L277" t="inlineStr">
         <is>
-          <t>#e1e221</t>
+          <t>#21e2e1</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="L278" t="inlineStr">
         <is>
-          <t>#bad726</t>
+          <t>#26d7ba</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="L279" t="inlineStr">
         <is>
-          <t>#9cb623</t>
+          <t>#23b69c</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="L280" t="inlineStr">
         <is>
-          <t>#a89411</t>
+          <t>#1194a8</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="L281" t="inlineStr">
         <is>
-          <t>#a38f1a</t>
+          <t>#1a8fa3</t>
         </is>
       </c>
     </row>
@@ -3203,140 +3203,140 @@
       </c>
       <c r="L282" t="inlineStr">
         <is>
-          <t>#cfc623</t>
+          <t>#23c6cf</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="L283" t="inlineStr">
         <is>
-          <t>#e7da02</t>
+          <t>#02dae7</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="L284" t="inlineStr">
         <is>
-          <t>#9e9407</t>
+          <t>#07949e</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="L285" t="inlineStr">
         <is>
-          <t>#c7c202</t>
+          <t>#02c2c7</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="L286" t="inlineStr">
         <is>
-          <t>#cdc702</t>
+          <t>#02c7cd</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="L287" t="inlineStr">
         <is>
-          <t>#d1c807</t>
+          <t>#07c8d1</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="L288" t="inlineStr">
         <is>
-          <t>#bbb701</t>
+          <t>#01b7bb</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="L289" t="inlineStr">
         <is>
-          <t>#d4cd01</t>
+          <t>#01cdd4</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="L290" t="inlineStr">
         <is>
-          <t>#eadf01</t>
+          <t>#01dfea</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="L291" t="inlineStr">
         <is>
-          <t>#d6d202</t>
+          <t>#02d2d6</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="L292" t="inlineStr">
         <is>
-          <t>#c6c101</t>
+          <t>#01c1c6</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="L293" t="inlineStr">
         <is>
-          <t>#d5cd08</t>
+          <t>#08cdd5</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="L294" t="inlineStr">
         <is>
-          <t>#837608</t>
+          <t>#087683</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="L295" t="inlineStr">
         <is>
-          <t>#867d00</t>
+          <t>#007d86</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="L296" t="inlineStr">
         <is>
-          <t>#d8d105</t>
+          <t>#05d1d8</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="L297" t="inlineStr">
         <is>
-          <t>#e5da02</t>
+          <t>#02dae5</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="L298" t="inlineStr">
         <is>
-          <t>#c1bd00</t>
+          <t>#00bdc1</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="L299" t="inlineStr">
         <is>
-          <t>#ece502</t>
+          <t>#02e5ec</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="L300" t="inlineStr">
         <is>
-          <t>#bab502</t>
+          <t>#02b5ba</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="L301" t="inlineStr">
         <is>
-          <t>#897e04</t>
+          <t>#047e89</t>
         </is>
       </c>
     </row>
@@ -3398,140 +3398,140 @@
       </c>
       <c r="L302" t="inlineStr">
         <is>
-          <t>#179e30</t>
+          <t>#309e17</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="L303" t="inlineStr">
         <is>
-          <t>#01a125</t>
+          <t>#25a101</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="L304" t="inlineStr">
         <is>
-          <t>#00991c</t>
+          <t>#1c9900</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="L305" t="inlineStr">
         <is>
-          <t>#02aa22</t>
+          <t>#22aa02</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="L306" t="inlineStr">
         <is>
-          <t>#03b026</t>
+          <t>#26b003</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="L307" t="inlineStr">
         <is>
-          <t>#036d14</t>
+          <t>#146d03</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="L308" t="inlineStr">
         <is>
-          <t>#0a5118</t>
+          <t>#18510a</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="L309" t="inlineStr">
         <is>
-          <t>#0d7c1a</t>
+          <t>#1a7c0d</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="L310" t="inlineStr">
         <is>
-          <t>#06871c</t>
+          <t>#1c8706</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="L311" t="inlineStr">
         <is>
-          <t>#083d0b</t>
+          <t>#0b3d08</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="L312" t="inlineStr">
         <is>
-          <t>#006d11</t>
+          <t>#116d00</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="L313" t="inlineStr">
         <is>
-          <t>#066816</t>
+          <t>#166806</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="L314" t="inlineStr">
         <is>
-          <t>#099523</t>
+          <t>#239509</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="L315" t="inlineStr">
         <is>
-          <t>#049a22</t>
+          <t>#229a04</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="L316" t="inlineStr">
         <is>
-          <t>#17741f</t>
+          <t>#1f7417</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="L317" t="inlineStr">
         <is>
-          <t>#05751d</t>
+          <t>#1d7505</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="L318" t="inlineStr">
         <is>
-          <t>#125714</t>
+          <t>#145712</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="L319" t="inlineStr">
         <is>
-          <t>#006811</t>
+          <t>#116800</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="L320" t="inlineStr">
         <is>
-          <t>#00ac22</t>
+          <t>#22ac00</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="L321" t="inlineStr">
         <is>
-          <t>#02a924</t>
+          <t>#24a902</t>
         </is>
       </c>
     </row>
@@ -3593,140 +3593,140 @@
       </c>
       <c r="L322" t="inlineStr">
         <is>
-          <t>#059e31</t>
+          <t>#319e05</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="L323" t="inlineStr">
         <is>
-          <t>#00a429</t>
+          <t>#29a400</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="L324" t="inlineStr">
         <is>
-          <t>#079a2c</t>
+          <t>#2c9a07</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="L325" t="inlineStr">
         <is>
-          <t>#0b9145</t>
+          <t>#45910b</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="L326" t="inlineStr">
         <is>
-          <t>#16944c</t>
+          <t>#4c9416</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="L327" t="inlineStr">
         <is>
-          <t>#257a46</t>
+          <t>#467a25</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="L328" t="inlineStr">
         <is>
-          <t>#0b7b3b</t>
+          <t>#3b7b0b</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="L329" t="inlineStr">
         <is>
-          <t>#00711e</t>
+          <t>#1e7100</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="L330" t="inlineStr">
         <is>
-          <t>#08651a</t>
+          <t>#1a6508</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="L331" t="inlineStr">
         <is>
-          <t>#089625</t>
+          <t>#259608</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="L332" t="inlineStr">
         <is>
-          <t>#03991d</t>
+          <t>#1d9903</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="L333" t="inlineStr">
         <is>
-          <t>#0a8b1e</t>
+          <t>#1e8b0a</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="L334" t="inlineStr">
         <is>
-          <t>#176e18</t>
+          <t>#186e17</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="L335" t="inlineStr">
         <is>
-          <t>#1d5f18</t>
+          <t>#185f1d</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="L336" t="inlineStr">
         <is>
-          <t>#017522</t>
+          <t>#227501</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="L337" t="inlineStr">
         <is>
-          <t>#045026</t>
+          <t>#265004</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="L338" t="inlineStr">
         <is>
-          <t>#144a2d</t>
+          <t>#2d4a14</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="L339" t="inlineStr">
         <is>
-          <t>#1f6e3d</t>
+          <t>#3d6e1f</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="L340" t="inlineStr">
         <is>
-          <t>#018629</t>
+          <t>#298601</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="L341" t="inlineStr">
         <is>
-          <t>#05a22f</t>
+          <t>#2fa205</t>
         </is>
       </c>
     </row>
@@ -3788,21 +3788,21 @@
       </c>
       <c r="L342" t="inlineStr">
         <is>
-          <t>#4ac54d</t>
+          <t>#4dc54a</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="L343" t="inlineStr">
         <is>
-          <t>#006f02</t>
+          <t>#026f00</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="L344" t="inlineStr">
         <is>
-          <t>#2c810d</t>
+          <t>#0d812c</t>
         </is>
       </c>
     </row>
@@ -3830,101 +3830,102 @@
     <row r="348">
       <c r="L348" t="inlineStr">
         <is>
-          <t>#27ac3e</t>
+          <t>#3eac27</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="L349" t="inlineStr">
         <is>
-          <t>#30a445</t>
+          <t>#45a430</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="L350" t="inlineStr">
         <is>
-          <t>#006a02</t>
+          <t>#026a00</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="L351" t="inlineStr">
         <is>
-          <t>#196400</t>
+          <t>#006419</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="L352" t="inlineStr">
         <is>
-          <t>#598306</t>
+          <t>#068359</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="L353" t="inlineStr">
         <is>
-          <t>#477f18</t>
+          <t>#187f47</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="L354" t="inlineStr">
         <is>
-          <t>#0a7e13</t>
+          <t>#137e0a</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="L355" t="inlineStr">
         <is>
-          <t>#007f15</t>
+          <t>#157f00</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="L356" t="inlineStr">
         <is>
-          <t>#221300</t>
+          <t>#001322</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="L357" t="inlineStr">
         <is>
-          <t>#3d4f00</t>
+          <t>#004f3d</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="L358" t="inlineStr">
         <is>
-          <t>#617514</t>
+          <t>#147561</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="L359" t="inlineStr">
         <is>
-          <t>#096f03</t>
+          <t>#036f09</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="L360" t="inlineStr">
         <is>
-          <t>#3c6d0b</t>
+          <t>#0b6d3c</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="L361" t="inlineStr">
         <is>
-          <t>#006e06</t>
-        </is>
-      </c>
-    </row>
+          <t>#066e00</t>
+        </is>
+      </c>
+    </row>
+    <row r="362"/>
   </sheetData>
   <mergeCells count="198">
     <mergeCell ref="A2:A21"/>

</xml_diff>